<commit_message>
correct cox related CI method
</commit_message>
<xml_diff>
--- a/vaccine_details.xlsx
+++ b/vaccine_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\COVID19-VaccinePhase3MetaAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8731258-5391-412E-818D-B1F684940958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489A911A-5C8E-46FB-B783-0E01D498140D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4815" yWindow="-18120" windowWidth="27405" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,9 +337,6 @@
     <t>Argentina, Chile, Mexico. Pakistan and russia</t>
   </si>
   <si>
-    <t>Binomial exact</t>
-  </si>
-  <si>
     <t>Halperin2021_Final_efficacy_analysis_interim_safety_analysis_and</t>
   </si>
   <si>
@@ -546,8 +543,11 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>Stratified Cox proportional-hazards model with Efron's method of tie handling</t>
+    <t>Stratified Cox proportional hazards model</t>
     <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cox proportional hazards model</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomRight" activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1486,7 +1486,7 @@
         <v>55</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>31</v>
@@ -1495,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X8" s="3"/>
     </row>
@@ -1554,7 +1554,7 @@
         <v>55</v>
       </c>
       <c r="T9" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>31</v>
@@ -1563,7 +1563,7 @@
         <v>32</v>
       </c>
       <c r="W9" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X9" s="3"/>
     </row>
@@ -1622,7 +1622,7 @@
         <v>55</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U10" s="3" t="s">
         <v>31</v>
@@ -1631,7 +1631,7 @@
         <v>32</v>
       </c>
       <c r="W10" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X10" s="3"/>
     </row>
@@ -1692,7 +1692,7 @@
         <v>55</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>31</v>
@@ -1758,7 +1758,7 @@
         <v>55</v>
       </c>
       <c r="T12" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U12" s="3" t="s">
         <v>31</v>
@@ -2754,7 +2754,7 @@
         <v>55</v>
       </c>
       <c r="T27" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U27" s="3" t="s">
         <v>92</v>
@@ -2820,7 +2820,7 @@
         <v>55</v>
       </c>
       <c r="T28" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U28" s="3" t="s">
         <v>92</v>
@@ -2886,7 +2886,7 @@
         <v>55</v>
       </c>
       <c r="T29" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U29" s="3" t="s">
         <v>92</v>
@@ -3084,7 +3084,7 @@
         <v>55</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="U32" s="3" t="s">
         <v>31</v>
@@ -3093,7 +3093,7 @@
         <v>32</v>
       </c>
       <c r="W32" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z32" s="1"/>
     </row>
@@ -3140,7 +3140,7 @@
         <v>100</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q33" s="3" t="s">
         <v>28</v>
@@ -3150,7 +3150,7 @@
         <v>55</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="U33" s="3" t="s">
         <v>31</v>
@@ -3159,7 +3159,7 @@
         <v>32</v>
       </c>
       <c r="W33" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z33" s="1"/>
     </row>
@@ -3216,7 +3216,7 @@
         <v>55</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="U34" s="3" t="s">
         <v>31</v>
@@ -3225,7 +3225,7 @@
         <v>32</v>
       </c>
       <c r="W34" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Z34" s="1"/>
     </row>
@@ -3263,13 +3263,13 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N35" s="5">
         <v>112</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P35" s="5" t="s">
         <v>43</v>
@@ -3291,7 +3291,7 @@
         <v>32</v>
       </c>
       <c r="W35" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X35" s="1"/>
     </row>
@@ -3329,16 +3329,16 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N36" s="5">
         <v>112</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>28</v>
@@ -3357,7 +3357,7 @@
         <v>32</v>
       </c>
       <c r="W36" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X36" s="1"/>
     </row>
@@ -3395,16 +3395,16 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N37" s="5">
         <v>112</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q37" s="3" t="s">
         <v>50</v>
@@ -3423,7 +3423,7 @@
         <v>32</v>
       </c>
       <c r="W37" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X37" s="1"/>
     </row>
@@ -3461,19 +3461,19 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N38" s="5">
         <v>112</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R38" s="3"/>
       <c r="S38" s="5" t="s">
@@ -3489,7 +3489,7 @@
         <v>32</v>
       </c>
       <c r="W38" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X38" s="1"/>
     </row>
@@ -3527,19 +3527,19 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N39" s="5">
         <v>112</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R39" s="3"/>
       <c r="S39" s="5" t="s">
@@ -3555,7 +3555,7 @@
         <v>32</v>
       </c>
       <c r="W39" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X39" s="1"/>
     </row>
@@ -3593,19 +3593,19 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N40" s="5">
         <v>112</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P40" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q40" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="R40" s="3"/>
       <c r="S40" s="5" t="s">
@@ -3621,7 +3621,7 @@
         <v>32</v>
       </c>
       <c r="W40" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="X40" s="1"/>
     </row>
@@ -3659,16 +3659,16 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N41" s="5">
         <v>28</v>
       </c>
       <c r="O41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="P41" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="P41" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>28</v>
@@ -3678,21 +3678,21 @@
         <v>44</v>
       </c>
       <c r="T41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="U41" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="U41" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="V41" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W41" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>24</v>
@@ -3730,10 +3730,10 @@
         <v>23</v>
       </c>
       <c r="O42" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P42" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>28</v>
@@ -3749,15 +3749,15 @@
         <v>31</v>
       </c>
       <c r="V42" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W42" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>24</v>
@@ -3795,7 +3795,7 @@
         <v>23</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P43" s="5" t="s">
         <v>94</v>
@@ -3814,15 +3814,15 @@
         <v>31</v>
       </c>
       <c r="V43" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W43" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>24</v>
@@ -3860,13 +3860,13 @@
         <v>23</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R44" s="3"/>
       <c r="S44" s="1" t="s">
@@ -3879,15 +3879,15 @@
         <v>31</v>
       </c>
       <c r="V44" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W44" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>24</v>
@@ -3925,10 +3925,10 @@
         <v>23</v>
       </c>
       <c r="O45" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P45" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="P45" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="Q45" s="3" t="s">
         <v>28</v>
@@ -3944,15 +3944,15 @@
         <v>31</v>
       </c>
       <c r="V45" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W45" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>24</v>
@@ -3990,7 +3990,7 @@
         <v>23</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P46" s="5" t="s">
         <v>94</v>
@@ -4009,15 +4009,15 @@
         <v>31</v>
       </c>
       <c r="V46" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W46" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>24</v>
@@ -4055,13 +4055,13 @@
         <v>23</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R47" s="3"/>
       <c r="S47" s="1" t="s">
@@ -4074,10 +4074,10 @@
         <v>31</v>
       </c>
       <c r="V47" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W47" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4121,10 +4121,10 @@
         <v>26</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R48" s="3"/>
       <c r="S48" s="3" t="s">
@@ -4134,13 +4134,13 @@
         <v>30</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V48" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W48" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X48" s="5">
         <v>18</v>
@@ -4200,13 +4200,13 @@
         <v>30</v>
       </c>
       <c r="U49" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W49" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4214,7 +4214,7 @@
         <v>23</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C50" s="5">
         <v>100</v>
@@ -4250,10 +4250,10 @@
         <v>26</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R50" s="3"/>
       <c r="S50" s="3" t="s">
@@ -4263,18 +4263,18 @@
         <v>30</v>
       </c>
       <c r="U50" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V50" s="3" t="s">
         <v>32</v>
       </c>
       <c r="W50" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>24</v>
@@ -4306,40 +4306,40 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N51" s="5">
         <v>227</v>
       </c>
       <c r="O51" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="P51" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="P51" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R51" s="5"/>
       <c r="S51" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U51" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="T51" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="U51" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="V51" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W51" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>24</v>
@@ -4371,35 +4371,35 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N52" s="5">
         <v>227</v>
       </c>
       <c r="O52" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="P52" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="P52" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="Q52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R52" s="5"/>
       <c r="S52" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U52" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="T52" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="U52" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W52" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4437,13 +4437,13 @@
         <v>90</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R53" s="5"/>
       <c r="S53" s="1" t="s">
@@ -4453,13 +4453,13 @@
         <v>61</v>
       </c>
       <c r="U53" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V53" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W53" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="V53" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="W53" s="16" t="s">
-        <v>136</v>
       </c>
       <c r="X53" s="5">
         <v>20</v>
@@ -4500,13 +4500,13 @@
         <v>90</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q54" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R54" s="5"/>
       <c r="S54" s="1" t="s">
@@ -4516,13 +4516,13 @@
         <v>61</v>
       </c>
       <c r="U54" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V54" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W54" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="V54" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="W54" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4560,10 +4560,10 @@
         <v>90</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>39</v>
@@ -4576,13 +4576,13 @@
         <v>61</v>
       </c>
       <c r="U55" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V55" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W55" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="V55" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="W55" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4620,13 +4620,13 @@
         <v>90</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P56" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q56" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R56" s="5"/>
       <c r="S56" s="1" t="s">
@@ -4636,13 +4636,13 @@
         <v>61</v>
       </c>
       <c r="U56" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V56" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="W56" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="V56" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="W56" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4650,7 +4650,7 @@
         <v>79</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" s="5">
         <v>70.400000000000006</v>
@@ -4679,7 +4679,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N57" s="5">
         <v>82</v>
@@ -4700,13 +4700,13 @@
         <v>61</v>
       </c>
       <c r="U57" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W57" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X57" s="5">
         <v>21</v>
@@ -4717,7 +4717,7 @@
         <v>79</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C58" s="5">
         <v>81.5</v>
@@ -4746,7 +4746,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N58" s="5">
         <v>82</v>
@@ -4767,18 +4767,18 @@
         <v>61</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V58" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W58" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>24</v>
@@ -4814,7 +4814,7 @@
         <v>365</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P59" s="5" t="s">
         <v>28</v>
@@ -4826,24 +4826,24 @@
         <v>1</v>
       </c>
       <c r="S59" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T59" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U59" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W59" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>24</v>
@@ -4878,10 +4878,10 @@
         <v>365</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P60" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q60" s="5" t="s">
         <v>50</v>
@@ -4890,24 +4890,24 @@
         <v>1</v>
       </c>
       <c r="S60" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T60" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U60" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V60" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W60" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>24</v>
@@ -4942,36 +4942,36 @@
         <v>365</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q61" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R61" s="5">
         <v>1</v>
       </c>
       <c r="S61" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T61" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U61" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V61" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W61" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>77</v>
@@ -5006,10 +5006,10 @@
         <v>365</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q62" s="5" t="s">
         <v>28</v>
@@ -5018,27 +5018,27 @@
         <v>1</v>
       </c>
       <c r="S62" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T62" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U62" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W62" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C63" s="5">
         <v>88.3</v>
@@ -5070,10 +5070,10 @@
         <v>365</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P63" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q63" s="5" t="s">
         <v>28</v>
@@ -5082,24 +5082,24 @@
         <v>1</v>
       </c>
       <c r="S63" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T63" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U63" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W63" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>78</v>
@@ -5134,10 +5134,10 @@
         <v>365</v>
       </c>
       <c r="O64" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q64" s="5" t="s">
         <v>28</v>
@@ -5146,24 +5146,24 @@
         <v>1</v>
       </c>
       <c r="S64" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T64" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U64" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V64" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W64" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>76</v>
@@ -5198,10 +5198,10 @@
         <v>365</v>
       </c>
       <c r="O65" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P65" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q65" s="5" t="s">
         <v>28</v>
@@ -5210,24 +5210,24 @@
         <v>1</v>
       </c>
       <c r="S65" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T65" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U65" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W65" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>24</v>
@@ -5256,13 +5256,13 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
       <c r="M66" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N66" s="5">
         <v>171</v>
       </c>
       <c r="O66" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P66" s="5" t="s">
         <v>28</v>
@@ -5274,24 +5274,24 @@
         <v>1</v>
       </c>
       <c r="S66" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T66" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U66" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W66" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>24</v>
@@ -5320,13 +5320,13 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
       <c r="M67" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N67" s="5">
         <v>171</v>
       </c>
       <c r="O67" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P67" s="5" t="s">
         <v>48</v>
@@ -5338,24 +5338,24 @@
         <v>1</v>
       </c>
       <c r="S67" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T67" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U67" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V67" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W67" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>24</v>
@@ -5384,13 +5384,13 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
       <c r="M68" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N68" s="5">
         <v>171</v>
       </c>
       <c r="O68" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>39</v>
@@ -5402,24 +5402,24 @@
         <v>1</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T68" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U68" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V68" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W68" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>76</v>
@@ -5451,7 +5451,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
       <c r="M69" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N69" s="5">
         <v>158</v>
@@ -5469,19 +5469,19 @@
         <v>1</v>
       </c>
       <c r="S69" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U69" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="U69" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W69" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X69" s="5">
         <v>24</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="70" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>76</v>
@@ -5523,7 +5523,7 @@
       <c r="M70" s="5"/>
       <c r="N70" s="5"/>
       <c r="O70" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P70" s="5" t="s">
         <v>28</v>
@@ -5535,19 +5535,19 @@
         <v>1</v>
       </c>
       <c r="S70" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T70" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U70" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V70" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W70" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X70" s="5">
         <v>25</v>
@@ -5555,7 +5555,7 @@
     </row>
     <row r="71" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>24</v>
@@ -5593,7 +5593,7 @@
         <v>61</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>28</v>
@@ -5603,24 +5603,24 @@
       </c>
       <c r="R71" s="5"/>
       <c r="S71" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T71" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U71" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V71" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W71" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>24</v>
@@ -5658,7 +5658,7 @@
         <v>61</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P72" s="5" t="s">
         <v>48</v>
@@ -5667,24 +5667,24 @@
         <v>48</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T72" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U72" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V72" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W72" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>24</v>
@@ -5722,33 +5722,33 @@
         <v>61</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q73" s="5" t="s">
         <v>50</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T73" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U73" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V73" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W73" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>24</v>
@@ -5786,33 +5786,33 @@
         <v>61</v>
       </c>
       <c r="O74" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q74" s="5" t="s">
         <v>75</v>
       </c>
       <c r="S74" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T74" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U74" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V74" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W74" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>24</v>
@@ -5847,7 +5847,7 @@
     </row>
     <row r="76" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>24</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="77" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>24</v>
@@ -5917,7 +5917,7 @@
     </row>
     <row r="78" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>24</v>
@@ -5952,7 +5952,7 @@
     </row>
     <row r="79" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>24</v>
@@ -5987,7 +5987,7 @@
     </row>
     <row r="80" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>24</v>
@@ -6014,15 +6014,15 @@
         <v>28</v>
       </c>
       <c r="P80" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q80" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>76</v>
@@ -7199,7 +7199,7 @@
   <customSheetViews>
     <customSheetView guid="{DE1A636D-2FFA-4081-94BF-35B6A450A334}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A1066" xr:uid="{906903A4-5E56-4648-AB8C-18F9A44FE6F7}">
+      <autoFilter ref="A1:A1066" xr:uid="{3F84F3FA-9CCF-427F-9879-FC258B8BDE5E}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="Ad26.COV2.S*"/>

</xml_diff>

<commit_message>
correct all VE CI method
</commit_message>
<xml_diff>
--- a/vaccine_details.xlsx
+++ b/vaccine_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\COVID19-VaccinePhase3MetaAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB46690B-80B8-4CD3-A8C3-42BD4B8B5F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1B3DE5-FA66-4ED1-882C-863BA17890D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4815" yWindow="-18120" windowWidth="27405" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="187">
   <si>
     <t>Vaccine</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Baptista-Pike method</t>
   </si>
   <si>
-    <t>Logunov2021_safety_and_efficacy_SputnikV</t>
-  </si>
-  <si>
     <t>Severe</t>
   </si>
   <si>
@@ -274,306 +271,364 @@
     <t>Poisson regression with robust error variance</t>
   </si>
   <si>
+    <t>Novavax</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Heath2021_Efficacy_of_the_NVX-CoV2373</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Symptomatic Covid-19</t>
+  </si>
+  <si>
+    <t>Covid-19 illness</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Sahly2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
+  </si>
+  <si>
+    <t>Severe disease</t>
+  </si>
+  <si>
+    <t>27/12/2020</t>
+  </si>
+  <si>
+    <t>Infection</t>
+  </si>
+  <si>
+    <t>Ad5-nCOV</t>
+  </si>
+  <si>
+    <t>22/09/2020</t>
+  </si>
+  <si>
+    <t>Argentina, Chile, Mexico. Pakistan and russia</t>
+  </si>
+  <si>
+    <t>Halperin2021_Final_efficacy_analysis_interim_safety_analysis_and</t>
+  </si>
+  <si>
+    <t>Symptomatic infection-after 28 days</t>
+  </si>
+  <si>
+    <t>28/08/2020</t>
+  </si>
+  <si>
+    <t>US,Chile and Peru</t>
+  </si>
+  <si>
+    <t>Falsey2021_phase3_safety_and_efficacy_of_AZD1222</t>
+  </si>
+  <si>
+    <t>Symptomatic infection-CDC definition</t>
+  </si>
+  <si>
+    <t>Severe or critical</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Hospitalization</t>
+  </si>
+  <si>
+    <t>ICU admission</t>
+  </si>
+  <si>
+    <t>ICU</t>
+  </si>
+  <si>
+    <t>15/12/2020</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Covid-19 infection</t>
+  </si>
+  <si>
+    <t>Double sided Clopper-Pearson</t>
+  </si>
+  <si>
+    <t>Phase 3 clinical trial (12-15)</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Symptomatic SARS-CoV-2</t>
+  </si>
+  <si>
+    <t>Pre-print</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>Documented infection</t>
+  </si>
+  <si>
+    <t>Post Phase 3 study</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>AZD1222*</t>
+  </si>
+  <si>
+    <t>23/04/2020</t>
+  </si>
+  <si>
+    <t>UK, Brazil, South africa</t>
+  </si>
+  <si>
+    <t>Symptotic Covid-19</t>
+  </si>
+  <si>
+    <t>1- adj relative risk</t>
+  </si>
+  <si>
+    <t>Booster-dose</t>
+  </si>
+  <si>
+    <t>Voysey2021_Single-dose_administration_and_the_influence</t>
+  </si>
+  <si>
+    <t>31/05/2020</t>
+  </si>
+  <si>
+    <t>Emary2021_Efficacy of ChAdOx1 nCoV-19 (AZD1222) vaccine against</t>
+  </si>
+  <si>
+    <t>Non beta</t>
+  </si>
+  <si>
+    <t>ZF2001</t>
+  </si>
+  <si>
+    <t>Uzbekistan, Pakistan, Indonesia and Ecuador</t>
+  </si>
+  <si>
+    <t>1 - Incidence rate ratio</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>Dai2022_efficacy_and_safety_of_the_RBD-Dimer-based</t>
+  </si>
+  <si>
+    <t>Severe-Critical</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>CoVLP</t>
+  </si>
+  <si>
+    <t>15/03/2021</t>
+  </si>
+  <si>
+    <t>Argentina, Brazil, Canada, Mexico, US and UK</t>
+  </si>
+  <si>
+    <t>Hager2022_Efficacy_and_Safety_of_a_recombiant_Plant</t>
+  </si>
+  <si>
+    <t>ZyCov-D</t>
+  </si>
+  <si>
+    <t>16/01/2021</t>
+  </si>
+  <si>
+    <t>BNT162b2*</t>
+  </si>
+  <si>
+    <t>Ad26.COV2.S*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium, Brazil, Coloumbia, France, Germany, Philippines, South africa, Spain, UK and US </t>
+  </si>
+  <si>
+    <t>Hardt2022_Efficacy_and_safety_of_a_booster_regimen</t>
+  </si>
+  <si>
+    <t>Asymptomatic Infection</t>
+  </si>
+  <si>
+    <t>All vaccine</t>
+  </si>
+  <si>
+    <t>SOBERANA-02</t>
+  </si>
+  <si>
+    <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+  </si>
+  <si>
+    <t>SOBERANA Plus</t>
+  </si>
+  <si>
+    <t>Palacios2021_CoronaVac_efficacy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wald test based on the Cox proportional hazards model</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stratified Cox proportional hazards model</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cox proportional hazards model</t>
+  </si>
+  <si>
+    <t>Bayesian beta-binomial model</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polack2020_safety_and_efficacy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-Odds ratio</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baden2021_efficacy_and_safety_mRNA_vaccine</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exact Poisson regression</t>
+  </si>
+  <si>
+    <t>Poisson regression</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dunkle2022_Efficacy_and_Safety_of_NVX_CoV_2373</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ella2021_efficacy_safety_and_lot_to_lot_immunogenicity_of_an_inactivated</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clopper-Pearson</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emary2021_Efficacy of ChAdOx1 nCoV-19 (AZD1222) vaccine against</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poisson regression with robust error variance</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Falsey2021_phase3_safety_and_efficacy_of_AZD1222</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dai2022_efficacy_and_safety_of_the_RBD-Dimer-based</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frenk2021_safety_immunogenicity_and_efficacy_of_the_BNT162b2</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hager2022_Efficacy_and_Safety_of_a_recombiant_Plant</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halperin2021_Final_efficacy_analysis_interim_safety_analysis_and</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hardt2022_Efficacy_and_safety_of_a_booster_regimen</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heath2021_Efficacy_of_the_NVX-CoV2373</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaabi2021_Effect_of_2_inactivated_SARS-CoV-2_vaccines_on_Symptomatic</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Khobragade2022_Efficacy_safety_and_immunogenicity_of_the_DNA_SAR</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logunov2021_safety_and_efficacy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baptista-Pike method</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moreira2022_Safety_and_efficacy_of_a_third_dose_of_BNT162b2.pdf</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double sided Clopper-Pearson</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sadoff2021_Safety_and_efficacy.pdf; https://www.fda.gov/media/146217/download</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sahly2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanriover2021_Efficacy_and_safety_of_an_inactivated_whole-virion</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-incidence rate ratio</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Person-time analysis</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thomas2021_Safety_and_Efficacy_of_the_BNT162b2_mRNA_Covid-19_vaccine_through_6_Months</t>
+  </si>
+  <si>
+    <t>Thomas2021_Safety_and_Efficacy_of_the_BNT162b2_mRNA_Covid-19_vaccine_through_6_Months</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
     <t>Voysey2021_Safety_and_efficacy_of</t>
-  </si>
-  <si>
-    <t>Novavax</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Heath2021_Efficacy_of_the_NVX-CoV2373</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>Symptomatic Covid-19</t>
-  </si>
-  <si>
-    <t>Events per COVID-19- free person-years</t>
-  </si>
-  <si>
-    <t>Tanriover2021_Efficacy_and_safety_of_an_inactivated_whole-virion</t>
-  </si>
-  <si>
-    <t>Covid-19 illness</t>
-  </si>
-  <si>
-    <t>Phase 4</t>
-  </si>
-  <si>
-    <t>Sahly2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
-  </si>
-  <si>
-    <t>Severe disease</t>
-  </si>
-  <si>
-    <t>27/12/2020</t>
-  </si>
-  <si>
-    <t>Infection</t>
-  </si>
-  <si>
-    <t>Ad5-nCOV</t>
-  </si>
-  <si>
-    <t>22/09/2020</t>
-  </si>
-  <si>
-    <t>Argentina, Chile, Mexico. Pakistan and russia</t>
-  </si>
-  <si>
-    <t>Halperin2021_Final_efficacy_analysis_interim_safety_analysis_and</t>
-  </si>
-  <si>
-    <t>Symptomatic infection-after 28 days</t>
-  </si>
-  <si>
-    <t>28/08/2020</t>
-  </si>
-  <si>
-    <t>US,Chile and Peru</t>
-  </si>
-  <si>
-    <t>Falsey2021_phase3_safety_and_efficacy_of_AZD1222</t>
-  </si>
-  <si>
-    <t>Symptomatic infection-CDC definition</t>
-  </si>
-  <si>
-    <t>Severe or critical</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>Hospitalization</t>
-  </si>
-  <si>
-    <t>ICU admission</t>
-  </si>
-  <si>
-    <t>ICU</t>
-  </si>
-  <si>
-    <t>15/12/2020</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Covid-19 infection</t>
-  </si>
-  <si>
-    <t>Double sided Clopper-Pearson</t>
-  </si>
-  <si>
-    <t>Phase 3 clinical trial (12-15)</t>
-  </si>
-  <si>
-    <t>Cuba</t>
-  </si>
-  <si>
-    <t>Symptomatic SARS-CoV-2</t>
-  </si>
-  <si>
-    <t>Pre-print</t>
-  </si>
-  <si>
-    <t>Death</t>
-  </si>
-  <si>
-    <t>Documented infection</t>
-  </si>
-  <si>
-    <t>Post Phase 3 study</t>
-  </si>
-  <si>
-    <t>Thomas2021_Six_month_safety_and_efficacy_of_the_BNT162b2</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>AZD1222*</t>
-  </si>
-  <si>
-    <t>23/04/2020</t>
-  </si>
-  <si>
-    <t>UK, Brazil, South africa</t>
-  </si>
-  <si>
-    <t>Symptotic Covid-19</t>
-  </si>
-  <si>
-    <t>1- adj relative risk</t>
-  </si>
-  <si>
-    <t>Booster-dose</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Voysey2021_Single-dose_administration_and_the_influence</t>
-  </si>
-  <si>
-    <t>31/05/2020</t>
-  </si>
-  <si>
-    <t>Emary2021_Efficacy of ChAdOx1 nCoV-19 (AZD1222) vaccine against</t>
-  </si>
-  <si>
-    <t>Non beta</t>
-  </si>
-  <si>
-    <t>ZF2001</t>
-  </si>
-  <si>
-    <t>Uzbekistan, Pakistan, Indonesia and Ecuador</t>
-  </si>
-  <si>
-    <t>1 - Incidence rate ratio</t>
-  </si>
-  <si>
-    <t>Phase 3</t>
-  </si>
-  <si>
-    <t>Dai2022_efficacy_and_safety_of_the_RBD-Dimer-based</t>
-  </si>
-  <si>
-    <t>Severe-Critical</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>CoVLP</t>
-  </si>
-  <si>
-    <t>15/03/2021</t>
-  </si>
-  <si>
-    <t>Argentina, Brazil, Canada, Mexico, US and UK</t>
-  </si>
-  <si>
-    <t>Hager2022_Efficacy_and_Safety_of_a_recombiant_Plant</t>
-  </si>
-  <si>
-    <t>ZyCov-D</t>
-  </si>
-  <si>
-    <t>16/01/2021</t>
-  </si>
-  <si>
-    <t>Khobragade2022_Efficacy_safety_and_immunogenicity_of_the_DNA_SAR</t>
-  </si>
-  <si>
-    <t>BNT162b2*</t>
-  </si>
-  <si>
-    <t>Moreira2022_Safety_and_efficacy_of_a_third_dose_of_BNT162b2.pdf</t>
-  </si>
-  <si>
-    <t>Ad26.COV2.S*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belgium, Brazil, Coloumbia, France, Germany, Philippines, South africa, Spain, UK and US </t>
-  </si>
-  <si>
-    <t>Hardt2022_Efficacy_and_safety_of_a_booster_regimen</t>
-  </si>
-  <si>
-    <t>Asymptomatic Infection</t>
-  </si>
-  <si>
-    <t>All vaccine</t>
-  </si>
-  <si>
-    <t>Robust Poisson model</t>
-  </si>
-  <si>
-    <t>SOBERANA-02</t>
-  </si>
-  <si>
-    <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
-  </si>
-  <si>
-    <t>SOBERANA Plus</t>
-  </si>
-  <si>
-    <t>Palacios2021_CoronaVac_efficacy</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wald test based on the Cox proportional hazards model</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stratified Cox proportional hazards model</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cox proportional hazards model</t>
-  </si>
-  <si>
-    <t>Bayesian beta-binomial model</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Polack2020_safety_and_efficacy</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-Odds ratio</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baden2021_efficacy_and_safety_mRNA_vaccine</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exact Poisson regression</t>
-  </si>
-  <si>
-    <t>Poisson regression</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dunkle2022_Efficacy_and_Safety_of_NVX_CoV_2373</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ella2021_efficacy_safety_and_lot_to_lot_immunogenicity_of_an_inactivated</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Clopper-Pearson</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emary2021_Efficacy of ChAdOx1 nCoV-19 (AZD1222) vaccine against</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poisson regression with robust error variance</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Falsey2021_phase3_safety_and_efficacy_of_AZD1222</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dai2022_efficacy_and_safety_of_the_RBD-Dimer-based</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Frenk2021_safety_immunogenicity_and_efficacy_of_the_BNT162b2</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hager2022_Efficacy_and_Safety_of_a_recombiant_Plant</t>
-    <phoneticPr fontId="13" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robust Poisson regression  model</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -584,7 +639,7 @@
     <numFmt numFmtId="176" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,21 +690,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -696,6 +739,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -730,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -747,19 +811,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -978,10 +1043,10 @@
   <dimension ref="A1:Z1062"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T28" sqref="T28"/>
+      <selection pane="bottomRight" activeCell="V76" sqref="V76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1078,7 +1143,7 @@
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>24</v>
@@ -1120,20 +1185,20 @@
         <v>88</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>31</v>
@@ -1141,13 +1206,13 @@
       <c r="V2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="19" t="s">
-        <v>163</v>
+      <c r="W2" s="17" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>24</v>
@@ -1156,10 +1221,10 @@
         <v>100</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="4">
         <v>15210</v>
@@ -1168,7 +1233,7 @@
         <v>15210</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="4">
         <v>30</v>
@@ -1185,20 +1250,20 @@
         <v>88</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R3" s="1"/>
       <c r="S3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>31</v>
@@ -1206,14 +1271,14 @@
       <c r="V3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="19" t="s">
-        <v>57</v>
+      <c r="W3" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>24</v>
@@ -1249,7 +1314,7 @@
         <v>365</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>28</v>
@@ -1261,19 +1326,19 @@
         <v>1</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W4" s="17" t="s">
-        <v>172</v>
+      <c r="W4" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="X4" s="1">
         <v>2</v>
@@ -1281,7 +1346,7 @@
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>24</v>
@@ -1316,37 +1381,37 @@
         <v>365</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R5" s="5">
         <v>1</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T5" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>24</v>
@@ -1381,40 +1446,40 @@
         <v>365</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="R6" s="5">
         <v>1</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T6" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W6" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="5">
         <v>76.099999999999994</v>
@@ -1446,10 +1511,10 @@
         <v>365</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="5" t="s">
         <v>28</v>
@@ -1458,28 +1523,28 @@
         <v>1</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T7" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C8" s="5">
         <v>88.3</v>
@@ -1511,10 +1576,10 @@
         <v>365</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>28</v>
@@ -1523,28 +1588,28 @@
         <v>1</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X8" s="3"/>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="5">
         <v>75.2</v>
@@ -1576,10 +1641,10 @@
         <v>365</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>28</v>
@@ -1588,28 +1653,28 @@
         <v>1</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T9" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W9" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="5">
         <v>71.900000000000006</v>
@@ -1641,10 +1706,10 @@
         <v>365</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>28</v>
@@ -1653,25 +1718,25 @@
         <v>1</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T10" s="18" t="s">
-        <v>165</v>
+        <v>128</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="X10" s="3"/>
     </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
@@ -1703,26 +1768,26 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N11" s="5">
         <v>53</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R11" s="3"/>
       <c r="S11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>31</v>
@@ -1730,14 +1795,14 @@
       <c r="V11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W11" s="20" t="s">
-        <v>166</v>
+      <c r="W11" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>24</v>
@@ -1769,26 +1834,26 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N12" s="5">
         <v>53</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="3"/>
       <c r="S12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U12" s="3" t="s">
         <v>31</v>
@@ -1796,14 +1861,14 @@
       <c r="V12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W12" s="20" t="s">
-        <v>166</v>
+      <c r="W12" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
@@ -1835,26 +1900,26 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N13" s="1">
         <v>52</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R13" s="5"/>
       <c r="S13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="T13" s="17" t="s">
-        <v>168</v>
+        <v>68</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="U13" s="3" t="s">
         <v>31</v>
@@ -1862,14 +1927,14 @@
       <c r="V13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W13" s="21" t="s">
-        <v>167</v>
+      <c r="W13" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>24</v>
@@ -1901,23 +1966,23 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N14" s="1">
         <v>52</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="5"/>
       <c r="S14" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T14" s="5" t="s">
         <v>30</v>
@@ -1929,13 +1994,13 @@
         <v>32</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>24</v>
@@ -1967,23 +2032,23 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N15" s="1">
         <v>52</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q15" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="Q15" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="R15" s="5"/>
       <c r="S15" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>30</v>
@@ -1995,16 +2060,16 @@
         <v>32</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4">
         <v>70.8</v>
@@ -2033,23 +2098,23 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N16" s="1">
         <v>52</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T16" s="5" t="s">
         <v>30</v>
@@ -2061,16 +2126,16 @@
         <v>32</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4">
         <v>65.2</v>
@@ -2099,23 +2164,23 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N17" s="1">
         <v>52</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R17" s="5"/>
       <c r="S17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>30</v>
@@ -2127,16 +2192,16 @@
         <v>32</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="4">
         <v>90.1</v>
@@ -2165,23 +2230,23 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N18" s="1">
         <v>52</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R18" s="5"/>
       <c r="S18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T18" s="5" t="s">
         <v>30</v>
@@ -2193,16 +2258,16 @@
         <v>32</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C19" s="5">
         <v>70.400000000000006</v>
@@ -2226,18 +2291,18 @@
         <v>40</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N19" s="5">
         <v>82</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>28</v>
@@ -2246,28 +2311,28 @@
         <v>28</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T19" s="18" t="s">
-        <v>165</v>
+        <v>41</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W19" s="17" t="s">
-        <v>169</v>
+      <c r="W19" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C20" s="5">
         <v>81.5</v>
@@ -2291,18 +2356,18 @@
         <v>80</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="N20" s="5">
         <v>82</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P20" s="5" t="s">
         <v>28</v>
@@ -2311,25 +2376,25 @@
         <v>28</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T20" s="18" t="s">
-        <v>165</v>
+        <v>41</v>
+      </c>
+      <c r="T20" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>24</v>
@@ -2361,26 +2426,26 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N21" s="5">
         <v>112</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R21" s="3"/>
       <c r="S21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T21" s="18" t="s">
-        <v>170</v>
+        <v>41</v>
+      </c>
+      <c r="T21" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>31</v>
@@ -2388,14 +2453,14 @@
       <c r="V21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W21" s="22" t="s">
-        <v>171</v>
+      <c r="W21" s="20" t="s">
+        <v>163</v>
       </c>
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>24</v>
@@ -2427,26 +2492,26 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N22" s="5">
         <v>112</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R22" s="3"/>
       <c r="S22" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T22" s="18" t="s">
-        <v>170</v>
+        <v>41</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="U22" s="3" t="s">
         <v>31</v>
@@ -2454,14 +2519,14 @@
       <c r="V22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W22" s="12" t="s">
-        <v>101</v>
+      <c r="W22" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>24</v>
@@ -2493,26 +2558,26 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N23" s="5">
         <v>112</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R23" s="3"/>
       <c r="S23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>31</v>
@@ -2520,14 +2585,14 @@
       <c r="V23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W23" s="12" t="s">
-        <v>101</v>
+      <c r="W23" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>24</v>
@@ -2559,26 +2624,26 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N24" s="5">
         <v>112</v>
       </c>
       <c r="O24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="P24" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P24" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="Q24" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>31</v>
@@ -2586,14 +2651,14 @@
       <c r="V24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W24" s="12" t="s">
-        <v>101</v>
+      <c r="W24" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>24</v>
@@ -2625,26 +2690,26 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N25" s="5">
         <v>112</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="R25" s="3"/>
       <c r="S25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T25" s="18" t="s">
-        <v>170</v>
+        <v>41</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="U25" s="3" t="s">
         <v>31</v>
@@ -2652,14 +2717,14 @@
       <c r="V25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W25" s="12" t="s">
-        <v>101</v>
+      <c r="W25" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>24</v>
@@ -2691,26 +2756,26 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N26" s="5">
         <v>112</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="R26" s="3"/>
       <c r="S26" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U26" s="3" t="s">
         <v>31</v>
@@ -2718,8 +2783,8 @@
       <c r="V26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W26" s="12" t="s">
-        <v>101</v>
+      <c r="W26" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="X26" s="1"/>
     </row>
@@ -2757,41 +2822,41 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N27" s="5">
         <v>28</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R27" s="3"/>
       <c r="S27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="V27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W27" s="22" t="s">
-        <v>173</v>
+      <c r="W27" s="20" t="s">
+        <v>165</v>
       </c>
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>24</v>
@@ -2820,13 +2885,13 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="N28" s="5">
         <v>171</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P28" s="5" t="s">
         <v>28</v>
@@ -2838,25 +2903,25 @@
         <v>1</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>164</v>
+        <v>128</v>
+      </c>
+      <c r="T28" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W28" s="17" t="s">
-        <v>174</v>
+      <c r="W28" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>24</v>
@@ -2885,43 +2950,43 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="N29" s="5">
         <v>171</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R29" s="5">
         <v>1</v>
       </c>
       <c r="S29" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>164</v>
+        <v>128</v>
+      </c>
+      <c r="T29" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U29" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V29" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W29" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>24</v>
@@ -2933,7 +2998,7 @@
         <v>-63.7</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="5">
         <v>12074</v>
@@ -2950,43 +3015,43 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="N30" s="5">
         <v>171</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R30" s="5">
         <v>1</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>164</v>
+        <v>128</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="U30" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V30" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W30" s="5" t="s">
-        <v>141</v>
+      <c r="W30" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>24</v>
@@ -3018,26 +3083,26 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N31" s="5">
         <v>115</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R31" s="3"/>
       <c r="S31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="U31" s="3" t="s">
         <v>31</v>
@@ -3045,14 +3110,14 @@
       <c r="V31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W31" s="12" t="s">
-        <v>97</v>
+      <c r="W31" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>24</v>
@@ -3084,26 +3149,26 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N32" s="5">
         <v>115</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R32" s="3"/>
       <c r="S32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="U32" s="3" t="s">
         <v>31</v>
@@ -3111,14 +3176,14 @@
       <c r="V32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W32" s="12" t="s">
-        <v>97</v>
+      <c r="W32" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>24</v>
@@ -3139,10 +3204,10 @@
         <v>14568</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J33" s="5">
         <v>6.5</v>
@@ -3150,26 +3215,26 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N33" s="5">
         <v>115</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R33" s="3"/>
       <c r="S33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="U33" s="3" t="s">
         <v>31</v>
@@ -3177,14 +3242,14 @@
       <c r="V33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W33" s="12" t="s">
-        <v>97</v>
+      <c r="W33" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>24</v>
@@ -3211,18 +3276,18 @@
         <v>53</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="P34" s="5" t="s">
         <v>28</v>
@@ -3232,25 +3297,25 @@
       </c>
       <c r="R34" s="5"/>
       <c r="S34" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U34" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="W34" s="5" t="s">
-        <v>149</v>
+        <v>111</v>
+      </c>
+      <c r="W34" s="15" t="s">
+        <v>168</v>
       </c>
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>24</v>
@@ -3277,45 +3342,45 @@
         <v>44</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U35" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V35" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="W35" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>24</v>
@@ -3342,45 +3407,45 @@
         <v>8</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O36" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="P36" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Q36" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S36" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U36" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V36" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="W36" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>24</v>
@@ -3407,45 +3472,45 @@
         <v>56</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="Q37" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U37" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V37" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="W37" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>24</v>
@@ -3477,26 +3542,26 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N38" s="5">
         <v>61</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q38" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R38" s="3"/>
       <c r="S38" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T38" s="17" t="s">
-        <v>170</v>
+        <v>41</v>
+      </c>
+      <c r="T38" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="U38" s="3" t="s">
         <v>31</v>
@@ -3504,17 +3569,17 @@
       <c r="V38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W38" s="5" t="s">
-        <v>83</v>
+      <c r="W38" s="15" t="s">
+        <v>169</v>
       </c>
       <c r="X38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="5">
         <v>86.3</v>
@@ -3526,16 +3591,16 @@
         <v>93.5</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J39" s="5">
         <v>2</v>
@@ -3543,26 +3608,26 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N39" s="5">
         <v>61</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R39" s="3"/>
       <c r="S39" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U39" s="3" t="s">
         <v>31</v>
@@ -3571,13 +3636,13 @@
         <v>32</v>
       </c>
       <c r="W39" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>24</v>
@@ -3613,16 +3678,16 @@
         <v>44.7</v>
       </c>
       <c r="M40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P40" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q40" s="3" t="s">
         <v>28</v>
@@ -3640,14 +3705,14 @@
       <c r="V40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W40" s="8" t="s">
-        <v>63</v>
+      <c r="W40" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="X40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>24</v>
@@ -3683,16 +3748,16 @@
         <v>44.7</v>
       </c>
       <c r="M41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P41" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>28</v>
@@ -3711,12 +3776,12 @@
         <v>32</v>
       </c>
       <c r="W41" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>24</v>
@@ -3725,10 +3790,10 @@
         <v>100</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F42" s="4">
         <v>13465</v>
@@ -3737,7 +3802,7 @@
         <v>13458</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I42" s="4">
         <v>2</v>
@@ -3748,19 +3813,19 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N42" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P42" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R42" s="3"/>
       <c r="S42" s="3" t="s">
@@ -3776,12 +3841,12 @@
         <v>32</v>
       </c>
       <c r="W42" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>24</v>
@@ -3790,10 +3855,10 @@
         <v>100</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F43" s="4">
         <v>13459</v>
@@ -3802,7 +3867,7 @@
         <v>13458</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I43" s="4">
         <v>2</v>
@@ -3813,19 +3878,19 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N43" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="P43" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R43" s="3"/>
       <c r="S43" s="3" t="s">
@@ -3841,15 +3906,15 @@
         <v>32</v>
       </c>
       <c r="W43" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="5">
         <v>66.599999999999994</v>
@@ -3878,13 +3943,13 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="N44" s="5">
         <v>158</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P44" s="5" t="s">
         <v>28</v>
@@ -3896,19 +3961,19 @@
         <v>1</v>
       </c>
       <c r="S44" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="V44" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W44" s="5" t="s">
-        <v>144</v>
+      <c r="W44" s="15" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -3960,11 +4025,11 @@
         <v>28</v>
       </c>
       <c r="R45" s="3"/>
-      <c r="S45" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="T45" s="3" t="s">
-        <v>35</v>
+      <c r="S45" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="T45" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="U45" s="3" t="s">
         <v>31</v>
@@ -3972,8 +4037,8 @@
       <c r="V45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W45" s="1" t="s">
-        <v>36</v>
+      <c r="W45" s="19" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4019,16 +4084,16 @@
         <v>34</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R46" s="3">
         <v>7</v>
       </c>
-      <c r="S46" s="18" t="s">
-        <v>162</v>
+      <c r="S46" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>35</v>
@@ -4039,16 +4104,16 @@
       <c r="V46" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W46" s="1" t="s">
-        <v>36</v>
+      <c r="W46" s="19" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="5">
         <v>94.8</v>
@@ -4079,7 +4144,7 @@
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>28</v>
@@ -4091,24 +4156,24 @@
         <v>1</v>
       </c>
       <c r="S47" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>111</v>
+        <v>128</v>
+      </c>
+      <c r="T47" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="U47" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W47" s="5" t="s">
-        <v>146</v>
+      <c r="W47" s="15" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>24</v>
@@ -4140,16 +4205,16 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N48" s="1">
         <v>148</v>
       </c>
       <c r="O48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P48" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P48" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>28</v>
@@ -4158,10 +4223,10 @@
         <v>2</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T48" s="17" t="s">
-        <v>157</v>
+        <v>51</v>
+      </c>
+      <c r="T48" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="U48" s="3" t="s">
         <v>31</v>
@@ -4169,8 +4234,8 @@
       <c r="V48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W48" s="16" t="s">
-        <v>156</v>
+      <c r="W48" s="14" t="s">
+        <v>148</v>
       </c>
       <c r="X48" s="5">
         <v>18</v>
@@ -4178,7 +4243,7 @@
     </row>
     <row r="49" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>24</v>
@@ -4210,28 +4275,28 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N49" s="1">
         <v>148</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R49" s="3">
         <v>4</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T49" s="17" t="s">
-        <v>157</v>
+        <v>51</v>
+      </c>
+      <c r="T49" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="U49" s="3" t="s">
         <v>31</v>
@@ -4239,13 +4304,13 @@
       <c r="V49" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W49" s="16" t="s">
-        <v>156</v>
+      <c r="W49" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>24</v>
@@ -4277,28 +4342,28 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N50" s="1">
         <v>148</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R50" s="3">
         <v>7</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T50" s="17" t="s">
-        <v>157</v>
+        <v>51</v>
+      </c>
+      <c r="T50" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="U50" s="3" t="s">
         <v>31</v>
@@ -4306,8 +4371,8 @@
       <c r="V50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W50" s="16" t="s">
-        <v>156</v>
+      <c r="W50" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4362,8 +4427,8 @@
       <c r="S51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T51" s="17" t="s">
-        <v>160</v>
+      <c r="T51" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="U51" s="3" t="s">
         <v>31</v>
@@ -4371,13 +4436,13 @@
       <c r="V51" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W51" s="18" t="s">
-        <v>161</v>
+      <c r="W51" s="16" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>24</v>
@@ -4406,43 +4471,43 @@
       <c r="J52" s="5">
         <v>2</v>
       </c>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14">
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12">
         <v>44411</v>
       </c>
       <c r="N52" s="5">
         <v>23</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P52" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Q52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R52" s="3"/>
       <c r="S52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T52" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T52" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U52" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V52" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W52" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W52" s="20" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>24</v>
@@ -4451,10 +4516,10 @@
         <v>63</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F53" s="5">
         <v>14371</v>
@@ -4471,38 +4536,38 @@
       <c r="J53" s="5">
         <v>2</v>
       </c>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14">
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12">
         <v>44411</v>
       </c>
       <c r="N53" s="5">
         <v>23</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R53" s="3"/>
       <c r="S53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T53" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T53" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V53" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W53" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W53" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="X53" s="5">
         <v>21</v>
@@ -4510,7 +4575,7 @@
     </row>
     <row r="54" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>24</v>
@@ -4519,10 +4584,10 @@
         <v>59</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F54" s="5">
         <v>14371</v>
@@ -4539,43 +4604,43 @@
       <c r="J54" s="5">
         <v>2</v>
       </c>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14">
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12">
         <v>44411</v>
       </c>
       <c r="N54" s="5">
         <v>23</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="R54" s="3"/>
       <c r="S54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T54" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T54" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U54" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V54" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W54" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W54" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>24</v>
@@ -4604,43 +4669,43 @@
       <c r="J55" s="5">
         <v>2</v>
       </c>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14">
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12">
         <v>44411</v>
       </c>
       <c r="N55" s="5">
         <v>23</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R55" s="3"/>
       <c r="S55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T55" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T55" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U55" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V55" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W55" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W55" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>24</v>
@@ -4649,10 +4714,10 @@
         <v>100</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F56" s="5">
         <v>13883</v>
@@ -4669,43 +4734,43 @@
       <c r="J56" s="5">
         <v>2</v>
       </c>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14">
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12">
         <v>44411</v>
       </c>
       <c r="N56" s="5">
         <v>23</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P56" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R56" s="3"/>
       <c r="S56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T56" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T56" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U56" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W56" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W56" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>24</v>
@@ -4714,10 +4779,10 @@
         <v>100</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F57" s="5">
         <v>13883</v>
@@ -4734,43 +4799,43 @@
       <c r="J57" s="5">
         <v>2</v>
       </c>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14">
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12">
         <v>44411</v>
       </c>
       <c r="N57" s="5">
         <v>23</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="R57" s="3"/>
       <c r="S57" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T57" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T57" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U57" s="3" t="s">
         <v>31</v>
       </c>
       <c r="V57" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W57" s="12" t="s">
-        <v>154</v>
+        <v>111</v>
+      </c>
+      <c r="W57" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>24</v>
@@ -4802,16 +4867,16 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N58" s="1">
         <v>123</v>
       </c>
       <c r="O58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P58" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q58" s="5" t="s">
         <v>28</v>
@@ -4820,10 +4885,10 @@
         <v>2</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T58" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U58" s="3" t="s">
         <v>31</v>
@@ -4831,13 +4896,13 @@
       <c r="V58" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W58" s="1" t="s">
-        <v>43</v>
+      <c r="W58" s="19" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>24</v>
@@ -4869,28 +4934,28 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N59" s="1">
         <v>123</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P59" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q59" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="Q59" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="R59" s="3">
         <v>4</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T59" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U59" s="3" t="s">
         <v>31</v>
@@ -4899,12 +4964,12 @@
         <v>32</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>24</v>
@@ -4936,26 +5001,26 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N60" s="1">
         <v>123</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q60" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="Q60" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="R60" s="3"/>
       <c r="S60" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T60" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="U60" s="3" t="s">
         <v>31</v>
@@ -4964,12 +5029,12 @@
         <v>32</v>
       </c>
       <c r="W60" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>24</v>
@@ -5007,34 +5072,34 @@
         <v>88</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="Q61" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R61" s="3"/>
       <c r="S61" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T61" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T61" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U61" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W61" s="13" t="s">
-        <v>90</v>
+      <c r="W61" s="22" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>24</v>
@@ -5072,34 +5137,34 @@
         <v>88</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q62" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R62" s="3"/>
       <c r="S62" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T62" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T62" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U62" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V62" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W62" s="12" t="s">
-        <v>90</v>
+      <c r="W62" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>24</v>
@@ -5137,34 +5202,34 @@
         <v>88</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P63" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q63" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="Q63" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="R63" s="3"/>
       <c r="S63" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T63" s="17" t="s">
-        <v>158</v>
+        <v>51</v>
+      </c>
+      <c r="T63" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="U63" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V63" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W63" s="12" t="s">
-        <v>90</v>
+      <c r="W63" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>24</v>
@@ -5200,20 +5265,20 @@
         <v>113</v>
       </c>
       <c r="O64" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P64" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q64" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R64" s="3"/>
-      <c r="S64" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T64" s="11" t="s">
-        <v>86</v>
+      <c r="S64" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="T64" s="23" t="s">
+        <v>181</v>
       </c>
       <c r="U64" s="3" t="s">
         <v>31</v>
@@ -5221,8 +5286,8 @@
       <c r="V64" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W64" s="12" t="s">
-        <v>87</v>
+      <c r="W64" s="20" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5266,26 +5331,26 @@
         <v>26</v>
       </c>
       <c r="P65" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q65" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="R65" s="3"/>
       <c r="S65" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T65" s="5" t="s">
-        <v>30</v>
+      <c r="T65" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="U65" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V65" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W65" s="12" t="s">
-        <v>119</v>
+      <c r="W65" s="20" t="s">
+        <v>183</v>
       </c>
       <c r="X65" s="5">
         <v>24</v>
@@ -5332,10 +5397,10 @@
         <v>26</v>
       </c>
       <c r="P66" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R66" s="3"/>
       <c r="S66" s="3" t="s">
@@ -5345,13 +5410,13 @@
         <v>30</v>
       </c>
       <c r="U66" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W66" s="12" t="s">
-        <v>119</v>
+      <c r="W66" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="X66" s="5">
         <v>25</v>
@@ -5362,7 +5427,7 @@
         <v>23</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C67" s="5">
         <v>100</v>
@@ -5380,10 +5445,10 @@
         <v>20794</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
@@ -5398,10 +5463,10 @@
         <v>26</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="R67" s="3"/>
       <c r="S67" s="3" t="s">
@@ -5411,18 +5476,18 @@
         <v>30</v>
       </c>
       <c r="U67" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="V67" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W67" s="12" t="s">
-        <v>119</v>
+      <c r="W67" s="11" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>24</v>
@@ -5454,26 +5519,26 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N68" s="1">
         <v>195</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q68" s="5" t="s">
         <v>28</v>
       </c>
       <c r="R68" s="3"/>
       <c r="S68" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>79</v>
+        <v>41</v>
+      </c>
+      <c r="T68" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="U68" s="3" t="s">
         <v>31</v>
@@ -5481,13 +5546,13 @@
       <c r="V68" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W68" s="1" t="s">
-        <v>80</v>
+      <c r="W68" s="19" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>24</v>
@@ -5519,40 +5584,40 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
       <c r="M69" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="N69" s="5">
         <v>227</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R69" s="5"/>
       <c r="S69" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>152</v>
+        <v>120</v>
+      </c>
+      <c r="T69" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="U69" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="W69" s="5" t="s">
-        <v>127</v>
+      <c r="W69" s="15" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>24</v>
@@ -5584,40 +5649,40 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
       <c r="M70" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="N70" s="5">
         <v>227</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Q70" s="3" t="s">
         <v>28</v>
       </c>
       <c r="R70" s="5"/>
       <c r="S70" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>152</v>
+        <v>120</v>
+      </c>
+      <c r="T70" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="U70" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V70" s="5" t="s">
         <v>32</v>
       </c>
       <c r="W70" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>24</v>
@@ -5652,7 +5717,7 @@
     </row>
     <row r="72" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>24</v>
@@ -5679,15 +5744,15 @@
         <v>587</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q72" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>24</v>
@@ -5714,15 +5779,15 @@
         <v>375</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q73" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>24</v>
@@ -5749,15 +5814,15 @@
         <v>230</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>24</v>
@@ -5784,15 +5849,15 @@
         <v>119</v>
       </c>
       <c r="P75" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q75" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>24</v>
@@ -5819,18 +5884,18 @@
         <v>28</v>
       </c>
       <c r="P76" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q76" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C77" s="5">
         <v>76.66</v>
@@ -5841,16 +5906,16 @@
       <c r="E77" s="5">
         <v>81.52</v>
       </c>
-      <c r="F77" s="15">
+      <c r="F77" s="13">
         <v>38502</v>
       </c>
-      <c r="G77" s="15">
+      <c r="G77" s="13">
         <v>38409</v>
       </c>
-      <c r="H77" s="15">
+      <c r="H77" s="13">
         <v>87</v>
       </c>
-      <c r="I77" s="15">
+      <c r="I77" s="13">
         <v>372</v>
       </c>
       <c r="P77" s="5" t="s">
@@ -5932,9 +5997,9 @@
     </row>
     <row r="96" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="97" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="K97" s="14"/>
-      <c r="L97" s="14"/>
-      <c r="M97" s="14"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
       <c r="Q97" s="5"/>
       <c r="R97" s="5"/>
       <c r="S97" s="5"/>
@@ -5943,9 +6008,9 @@
     </row>
     <row r="98" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1"/>
-      <c r="K98" s="14"/>
-      <c r="L98" s="14"/>
-      <c r="M98" s="14"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
       <c r="Q98" s="5"/>
       <c r="R98" s="5"/>
       <c r="S98" s="5"/>
@@ -5954,9 +6019,9 @@
     </row>
     <row r="99" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1"/>
-      <c r="K99" s="14"/>
-      <c r="L99" s="14"/>
-      <c r="M99" s="14"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
       <c r="Q99" s="5"/>
       <c r="R99" s="5"/>
       <c r="S99" s="5"/>
@@ -5965,9 +6030,9 @@
     </row>
     <row r="100" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1"/>
-      <c r="K100" s="14"/>
-      <c r="L100" s="14"/>
-      <c r="M100" s="14"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
+      <c r="M100" s="12"/>
       <c r="Q100" s="5"/>
       <c r="R100" s="5"/>
       <c r="S100" s="5"/>
@@ -5976,9 +6041,9 @@
     </row>
     <row r="101" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1"/>
-      <c r="K101" s="14"/>
-      <c r="L101" s="14"/>
-      <c r="M101" s="14"/>
+      <c r="K101" s="12"/>
+      <c r="L101" s="12"/>
+      <c r="M101" s="12"/>
       <c r="Q101" s="5"/>
       <c r="R101" s="5"/>
       <c r="S101" s="5"/>
@@ -6003,15 +6068,15 @@
       <c r="M104" s="10"/>
     </row>
     <row r="105" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="K105" s="14"/>
-      <c r="L105" s="14"/>
-      <c r="M105" s="14"/>
+      <c r="K105" s="12"/>
+      <c r="L105" s="12"/>
+      <c r="M105" s="12"/>
       <c r="Q105" s="3"/>
     </row>
     <row r="106" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
-      <c r="M106" s="14"/>
+      <c r="K106" s="12"/>
+      <c r="L106" s="12"/>
+      <c r="M106" s="12"/>
       <c r="Q106" s="3"/>
     </row>
     <row r="107" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -7008,7 +7073,7 @@
   <customSheetViews>
     <customSheetView guid="{DE1A636D-2FFA-4081-94BF-35B6A450A334}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A1066" xr:uid="{D02E020D-030C-49DF-AC9C-927999A4802C}">
+      <autoFilter ref="A1:A1066" xr:uid="{979A69CE-BBD4-4B80-969D-8A4750ACE166}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="Ad26.COV2.S*"/>
@@ -7035,7 +7100,7 @@
       </extLst>
     </customSheetView>
   </customSheetViews>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Update box plot to violin plot
</commit_message>
<xml_diff>
--- a/vaccine_details.xlsx
+++ b/vaccine_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\COVID19-VaccinePhase3MetaAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276D3454-DB1B-4BEE-B60C-4A95F24CE874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED23E7DF-A119-4B07-B9FC-33CCF39B70E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4815" yWindow="-18120" windowWidth="27405" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="187">
   <si>
     <t>Vaccine</t>
   </si>
@@ -482,10 +482,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Wald test based on the Cox proportional hazards model</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>Cox proportional hazards model</t>
   </si>
   <si>
@@ -624,6 +620,14 @@
   </si>
   <si>
     <t>Cox proportional hazards model</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wald</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1- adj relative risk</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -1039,10 +1043,10 @@
   <dimension ref="A1:Z1062"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1194,7 +1198,7 @@
         <v>51</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>31</v>
@@ -1203,7 +1207,7 @@
         <v>32</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -1259,7 +1263,7 @@
         <v>51</v>
       </c>
       <c r="T3" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>31</v>
@@ -1325,7 +1329,7 @@
         <v>128</v>
       </c>
       <c r="T4" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>129</v>
@@ -1334,7 +1338,7 @@
         <v>32</v>
       </c>
       <c r="W4" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X4" s="1">
         <v>2</v>
@@ -1392,7 +1396,7 @@
         <v>128</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>129</v>
@@ -1457,7 +1461,7 @@
         <v>128</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>129</v>
@@ -1522,7 +1526,7 @@
         <v>128</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>129</v>
@@ -1587,7 +1591,7 @@
         <v>128</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U8" s="5" t="s">
         <v>129</v>
@@ -1652,7 +1656,7 @@
         <v>128</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U9" s="5" t="s">
         <v>129</v>
@@ -1717,7 +1721,7 @@
         <v>128</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U10" s="5" t="s">
         <v>129</v>
@@ -1792,7 +1796,7 @@
         <v>32</v>
       </c>
       <c r="W11" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X11" s="1"/>
     </row>
@@ -1858,7 +1862,7 @@
         <v>32</v>
       </c>
       <c r="W12" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X12" s="1"/>
     </row>
@@ -1915,7 +1919,7 @@
         <v>68</v>
       </c>
       <c r="T13" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U13" s="3" t="s">
         <v>31</v>
@@ -1924,7 +1928,7 @@
         <v>32</v>
       </c>
       <c r="W13" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="X13" s="1"/>
     </row>
@@ -2310,7 +2314,7 @@
         <v>41</v>
       </c>
       <c r="T19" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U19" s="5" t="s">
         <v>114</v>
@@ -2319,7 +2323,7 @@
         <v>32</v>
       </c>
       <c r="W19" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X19" s="1"/>
     </row>
@@ -2337,7 +2341,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="E20" s="5">
-        <v>80.400000000000006</v>
+        <v>89.4</v>
       </c>
       <c r="F20" s="5">
         <v>4244</v>
@@ -2375,7 +2379,7 @@
         <v>41</v>
       </c>
       <c r="T20" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U20" s="5" t="s">
         <v>114</v>
@@ -2441,7 +2445,7 @@
         <v>41</v>
       </c>
       <c r="T21" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>31</v>
@@ -2450,7 +2454,7 @@
         <v>32</v>
       </c>
       <c r="W21" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X21" s="1"/>
     </row>
@@ -2507,7 +2511,7 @@
         <v>41</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U22" s="3" t="s">
         <v>31</v>
@@ -2516,7 +2520,7 @@
         <v>32</v>
       </c>
       <c r="W22" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X22" s="1"/>
     </row>
@@ -2573,7 +2577,7 @@
         <v>41</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>31</v>
@@ -2582,7 +2586,7 @@
         <v>32</v>
       </c>
       <c r="W23" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X23" s="1"/>
     </row>
@@ -2639,7 +2643,7 @@
         <v>41</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>31</v>
@@ -2705,7 +2709,7 @@
         <v>41</v>
       </c>
       <c r="T25" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U25" s="3" t="s">
         <v>31</v>
@@ -2771,7 +2775,7 @@
         <v>41</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U26" s="3" t="s">
         <v>31</v>
@@ -2846,7 +2850,7 @@
         <v>32</v>
       </c>
       <c r="W27" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X27" s="1"/>
     </row>
@@ -2902,7 +2906,7 @@
         <v>128</v>
       </c>
       <c r="T28" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U28" s="5" t="s">
         <v>129</v>
@@ -2911,7 +2915,7 @@
         <v>32</v>
       </c>
       <c r="W28" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X28" s="1"/>
     </row>
@@ -2967,7 +2971,7 @@
         <v>128</v>
       </c>
       <c r="T29" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U29" s="5" t="s">
         <v>129</v>
@@ -3032,7 +3036,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U30" s="5" t="s">
         <v>129</v>
@@ -3041,7 +3045,7 @@
         <v>32</v>
       </c>
       <c r="W30" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X30" s="1"/>
     </row>
@@ -3098,7 +3102,7 @@
         <v>51</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U31" s="3" t="s">
         <v>31</v>
@@ -3107,7 +3111,7 @@
         <v>32</v>
       </c>
       <c r="W31" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X31" s="1"/>
     </row>
@@ -3164,7 +3168,7 @@
         <v>51</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U32" s="3" t="s">
         <v>31</v>
@@ -3230,7 +3234,7 @@
         <v>51</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U33" s="3" t="s">
         <v>31</v>
@@ -3296,7 +3300,7 @@
         <v>128</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U34" s="5" t="s">
         <v>121</v>
@@ -3305,7 +3309,7 @@
         <v>111</v>
       </c>
       <c r="W34" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Z34" s="1"/>
     </row>
@@ -3361,7 +3365,7 @@
         <v>128</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U35" s="5" t="s">
         <v>121</v>
@@ -3426,7 +3430,7 @@
         <v>128</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U36" s="5" t="s">
         <v>121</v>
@@ -3491,7 +3495,7 @@
         <v>128</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U37" s="5" t="s">
         <v>121</v>
@@ -3557,7 +3561,7 @@
         <v>41</v>
       </c>
       <c r="T38" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U38" s="3" t="s">
         <v>31</v>
@@ -3566,7 +3570,7 @@
         <v>32</v>
       </c>
       <c r="W38" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X38" s="1"/>
     </row>
@@ -3702,7 +3706,7 @@
         <v>32</v>
       </c>
       <c r="W40" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X40" s="1"/>
     </row>
@@ -3969,7 +3973,7 @@
         <v>32</v>
       </c>
       <c r="W44" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4022,10 +4026,10 @@
       </c>
       <c r="R45" s="3"/>
       <c r="S45" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T45" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U45" s="3" t="s">
         <v>31</v>
@@ -4034,7 +4038,7 @@
         <v>32</v>
       </c>
       <c r="W45" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4089,7 +4093,7 @@
         <v>7</v>
       </c>
       <c r="S46" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>35</v>
@@ -4101,7 +4105,7 @@
         <v>32</v>
       </c>
       <c r="W46" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4155,7 +4159,7 @@
         <v>128</v>
       </c>
       <c r="T47" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U47" s="5" t="s">
         <v>121</v>
@@ -4164,7 +4168,7 @@
         <v>32</v>
       </c>
       <c r="W47" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4222,7 +4226,7 @@
         <v>51</v>
       </c>
       <c r="T48" s="15" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="U48" s="3" t="s">
         <v>31</v>
@@ -4292,7 +4296,7 @@
         <v>51</v>
       </c>
       <c r="T49" s="15" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="U49" s="3" t="s">
         <v>31</v>
@@ -4359,7 +4363,7 @@
         <v>51</v>
       </c>
       <c r="T50" s="15" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="U50" s="3" t="s">
         <v>31</v>
@@ -4424,7 +4428,7 @@
         <v>29</v>
       </c>
       <c r="T51" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U51" s="3" t="s">
         <v>31</v>
@@ -4433,7 +4437,7 @@
         <v>32</v>
       </c>
       <c r="W51" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4489,7 +4493,7 @@
         <v>51</v>
       </c>
       <c r="T52" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U52" s="3" t="s">
         <v>31</v>
@@ -4498,7 +4502,7 @@
         <v>111</v>
       </c>
       <c r="W52" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4554,7 +4558,7 @@
         <v>51</v>
       </c>
       <c r="T53" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U53" s="3" t="s">
         <v>31</v>
@@ -4622,7 +4626,7 @@
         <v>51</v>
       </c>
       <c r="T54" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U54" s="3" t="s">
         <v>31</v>
@@ -4687,7 +4691,7 @@
         <v>51</v>
       </c>
       <c r="T55" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U55" s="3" t="s">
         <v>31</v>
@@ -4752,7 +4756,7 @@
         <v>51</v>
       </c>
       <c r="T56" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U56" s="3" t="s">
         <v>31</v>
@@ -4817,7 +4821,7 @@
         <v>51</v>
       </c>
       <c r="T57" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U57" s="3" t="s">
         <v>31</v>
@@ -4884,7 +4888,7 @@
         <v>41</v>
       </c>
       <c r="T58" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U58" s="3" t="s">
         <v>31</v>
@@ -4893,7 +4897,7 @@
         <v>32</v>
       </c>
       <c r="W58" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4951,7 +4955,7 @@
         <v>41</v>
       </c>
       <c r="T59" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U59" s="3" t="s">
         <v>31</v>
@@ -5016,7 +5020,7 @@
         <v>41</v>
       </c>
       <c r="T60" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U60" s="3" t="s">
         <v>31</v>
@@ -5081,7 +5085,7 @@
         <v>51</v>
       </c>
       <c r="T61" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U61" s="3" t="s">
         <v>85</v>
@@ -5090,7 +5094,7 @@
         <v>32</v>
       </c>
       <c r="W61" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5146,7 +5150,7 @@
         <v>51</v>
       </c>
       <c r="T62" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U62" s="3" t="s">
         <v>85</v>
@@ -5211,7 +5215,7 @@
         <v>51</v>
       </c>
       <c r="T63" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U63" s="3" t="s">
         <v>85</v>
@@ -5271,10 +5275,10 @@
       </c>
       <c r="R64" s="3"/>
       <c r="S64" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="T64" s="23" t="s">
         <v>179</v>
-      </c>
-      <c r="T64" s="23" t="s">
-        <v>180</v>
       </c>
       <c r="U64" s="3" t="s">
         <v>31</v>
@@ -5283,7 +5287,7 @@
         <v>32</v>
       </c>
       <c r="W64" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5337,7 +5341,7 @@
         <v>29</v>
       </c>
       <c r="T65" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U65" s="3" t="s">
         <v>114</v>
@@ -5346,7 +5350,7 @@
         <v>32</v>
       </c>
       <c r="W65" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X65" s="5">
         <v>24</v>
@@ -5412,7 +5416,7 @@
         <v>32</v>
       </c>
       <c r="W66" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X66" s="5">
         <v>25</v>
@@ -5478,7 +5482,7 @@
         <v>32</v>
       </c>
       <c r="W67" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5534,7 +5538,7 @@
         <v>41</v>
       </c>
       <c r="T68" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U68" s="3" t="s">
         <v>31</v>
@@ -5543,7 +5547,7 @@
         <v>32</v>
       </c>
       <c r="W68" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5595,11 +5599,11 @@
         <v>28</v>
       </c>
       <c r="R69" s="5"/>
-      <c r="S69" s="5" t="s">
-        <v>120</v>
+      <c r="S69" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="T69" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U69" s="5" t="s">
         <v>121</v>
@@ -5608,7 +5612,7 @@
         <v>32</v>
       </c>
       <c r="W69" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -5664,7 +5668,7 @@
         <v>120</v>
       </c>
       <c r="T70" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U70" s="5" t="s">
         <v>121</v>
@@ -7069,7 +7073,7 @@
   <customSheetViews>
     <customSheetView guid="{DE1A636D-2FFA-4081-94BF-35B6A450A334}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:A1066" xr:uid="{CF0BEDC2-9DC7-494C-B281-DDC53F74261E}">
+      <autoFilter ref="A1:A1066" xr:uid="{90AB38B8-070C-46DE-BEDB-22963BD4FFF7}">
         <filterColumn colId="0">
           <filters blank="1">
             <filter val="Ad26.COV2.S*"/>

</xml_diff>